<commit_message>
add Page Recommend_Person_details&fix some bugs of TableBase&Add a view
2018/11/15 Second Commit

Author:tsz

- fix some problems of `TableBase`
- modify `TableBase` to allow no head Table.
- I have write a subclass of TableBase `Table_for_SRM_vOpen`，you may find how to write your subclass to fit it to your condition in it.
- add new view recommend_person_details
- fix the lack of column `rp_job` in table `recommend_people`
</commit_message>
<xml_diff>
--- a/table_details/table_details_all.xlsx
+++ b/table_details/table_details_all.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18C636C-CBD1-4F52-8271-5BB032453ECB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D557F012-0B6C-4B4F-A4B0-B00BBBE409CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-5" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="16-19" sheetId="8" r:id="rId4"/>
     <sheet name="20-23" sheetId="9" r:id="rId5"/>
     <sheet name="24-26" sheetId="10" r:id="rId6"/>
-    <sheet name="View(1-2)" sheetId="11" r:id="rId7"/>
+    <sheet name="View(1-3)" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="307">
   <si>
     <t>表名：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1379,6 +1379,18 @@
   </si>
   <si>
     <t>stf_jt_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>commend_person_details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rp_deg_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rp_uni_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1790,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2444,7 +2456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -2818,14 +2830,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92048D4E-400A-4C99-98D4-96FDDBC09EAE}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C23"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.625" customWidth="1"/>
     <col min="2" max="2" width="9.625" customWidth="1"/>
+    <col min="3" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -4570,10 +4591,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D6CB52-9EB7-455C-8F84-F35A52C5F1B4}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="B20" sqref="B20:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4583,7 +4604,7 @@
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>296</v>
       </c>
@@ -4591,7 +4612,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>129</v>
       </c>
@@ -4611,7 +4632,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>130</v>
       </c>
@@ -4631,7 +4652,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>131</v>
       </c>
@@ -4645,7 +4666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>132</v>
       </c>
@@ -4665,7 +4686,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>133</v>
       </c>
@@ -4685,7 +4706,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>296</v>
       </c>
@@ -4693,7 +4714,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -4704,7 +4725,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -4715,7 +4736,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -4723,7 +4744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -4734,7 +4755,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -4745,17 +4766,248 @@
         <v>303</v>
       </c>
     </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" t="s">
+        <v>153</v>
+      </c>
+      <c r="H16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I16" t="s">
+        <v>188</v>
+      </c>
+      <c r="J16" t="s">
+        <v>194</v>
+      </c>
+      <c r="K16" t="s">
+        <v>157</v>
+      </c>
+      <c r="L16" t="s">
+        <v>158</v>
+      </c>
+      <c r="M16" t="s">
+        <v>159</v>
+      </c>
+      <c r="N16" t="s">
+        <v>160</v>
+      </c>
+      <c r="O16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <v>20</v>
+      </c>
+      <c r="H18">
+        <v>20</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>20</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" t="s">
+        <v>167</v>
+      </c>
+      <c r="F20" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" t="s">
+        <v>169</v>
+      </c>
+      <c r="H20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I20" t="s">
+        <v>305</v>
+      </c>
+      <c r="J20" t="s">
+        <v>306</v>
+      </c>
+      <c r="K20" t="s">
+        <v>173</v>
+      </c>
+      <c r="L20" t="s">
+        <v>174</v>
+      </c>
+      <c r="M20" t="s">
+        <v>175</v>
+      </c>
+      <c r="N20" t="s">
+        <v>176</v>
+      </c>
+      <c r="O20" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:F3 B10:C10" xr:uid="{672A8DB7-17F9-4041-9274-565953294B28}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:F3 B10:C10 M17:O17 B17:K17" xr:uid="{672A8DB7-17F9-4041-9274-565953294B28}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:F5 B12" xr:uid="{46A27783-6485-4EF8-89C7-A4A0624C58E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:F5 B12 B19:O19" xr:uid="{46A27783-6485-4EF8-89C7-A4A0624C58E8}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{60417A34-0ECB-4D94-89CD-F63C40054958}">
       <formula1>"k,m,k&amp;m"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L17" xr:uid="{6BC1AFAF-92C1-4FFF-9FDF-59CE7671F298}">
+      <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Workflow class sample(Tsk_Sift,still unfinished)
- 添加了workflow函数类的样例:Tsk_Sift
- 添加了自动生成枚举类的python工具(in Tools)，并添加了许多必要的枚举类
- 修了一些问题(JobType class，table_details_all.xlsx
- 数据库脚本add_samples.sql有更新
</commit_message>
<xml_diff>
--- a/table_details/table_details_all.xlsx
+++ b/table_details/table_details_all.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D557F012-0B6C-4B4F-A4B0-B00BBBE409CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BDF987-72BB-490E-8F8D-6917B22FF9A6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-5" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="306">
   <si>
     <t>表名：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -729,10 +729,6 @@
   </si>
   <si>
     <t>处理结果表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>recommend_resluts</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1254,10 +1250,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>积分变化规则表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1391,6 +1383,10 @@
   </si>
   <si>
     <t>rp_uni_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recommend_results</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1802,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1993,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -2001,7 +1997,7 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -2009,10 +2005,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -2457,7 +2453,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2830,8 +2826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92048D4E-400A-4C99-98D4-96FDDBC09EAE}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3242,7 +3238,7 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
@@ -3250,10 +3246,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" t="s">
         <v>181</v>
-      </c>
-      <c r="C27" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
@@ -3291,10 +3287,10 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" t="s">
         <v>183</v>
-      </c>
-      <c r="C31" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -3302,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -3310,7 +3306,7 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -3318,10 +3314,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" t="s">
         <v>187</v>
-      </c>
-      <c r="C35" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -3359,10 +3355,10 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" t="s">
         <v>189</v>
-      </c>
-      <c r="C39" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3370,7 +3366,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -3378,7 +3374,7 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -3386,10 +3382,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43" t="s">
         <v>193</v>
-      </c>
-      <c r="C43" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -3427,10 +3423,10 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
+        <v>194</v>
+      </c>
+      <c r="C47" t="s">
         <v>195</v>
-      </c>
-      <c r="C47" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3454,8 +3450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D6809F-1A5A-41FB-870C-741234E0C666}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C16"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3475,7 +3471,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -3543,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D10" s="7"/>
     </row>
@@ -3552,7 +3548,7 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3560,28 +3556,28 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
         <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E12" t="s">
         <v>148</v>
       </c>
       <c r="F12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G12" t="s">
         <v>124</v>
       </c>
       <c r="H12" t="s">
+        <v>201</v>
+      </c>
+      <c r="I12" t="s">
         <v>202</v>
-      </c>
-      <c r="I12" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3652,28 +3648,28 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" t="s">
         <v>204</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>205</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>206</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>207</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>208</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>209</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>210</v>
-      </c>
-      <c r="I16" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -3681,7 +3677,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3689,7 +3685,7 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D20" s="7"/>
     </row>
@@ -3698,16 +3694,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" t="s">
         <v>214</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>215</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>216</v>
-      </c>
-      <c r="E21" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3754,16 +3750,16 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C25" t="s">
         <v>218</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>219</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>220</v>
-      </c>
-      <c r="E25" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3771,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -3779,7 +3775,7 @@
         <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3787,10 +3783,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3828,10 +3824,10 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" t="s">
         <v>225</v>
-      </c>
-      <c r="C33" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3853,7 +3849,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3874,7 +3870,7 @@
         <v>128</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C1" s="8"/>
     </row>
@@ -3883,7 +3879,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="11"/>
@@ -3894,10 +3890,10 @@
         <v>129</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="D3" s="11"/>
       <c r="F3" s="12"/>
@@ -3938,10 +3934,10 @@
         <v>133</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>231</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -3949,7 +3945,7 @@
         <v>128</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C10" s="8"/>
     </row>
@@ -3958,7 +3954,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" s="8"/>
     </row>
@@ -3967,34 +3963,34 @@
         <v>129</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="D12" s="17" t="s">
         <v>236</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>237</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>148</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G12" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="H12" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="I12" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="J12" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="K12" s="17" t="s">
         <v>241</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -4080,34 +4076,34 @@
         <v>133</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="F16" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="G16" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H16" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="I16" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="J16" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="K16" s="17" t="s">
         <v>251</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -4115,7 +4111,7 @@
         <v>128</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C19" s="8"/>
     </row>
@@ -4124,7 +4120,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C20" s="8"/>
     </row>
@@ -4133,10 +4129,10 @@
         <v>129</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F21" s="17"/>
       <c r="I21" s="17"/>
@@ -4177,10 +4173,10 @@
         <v>133</v>
       </c>
       <c r="B25" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>256</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>257</v>
       </c>
       <c r="E25" s="19"/>
     </row>
@@ -4192,7 +4188,7 @@
         <v>128</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C27" s="8"/>
     </row>
@@ -4201,7 +4197,7 @@
         <v>46</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C28" s="8"/>
     </row>
@@ -4210,13 +4206,13 @@
         <v>129</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C29" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="D29" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -4259,13 +4255,13 @@
         <v>133</v>
       </c>
       <c r="B33" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="D33" s="17" t="s">
         <v>263</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -4297,8 +4293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F506D6B7-3E6F-45FA-91C1-7913AE5D78D4}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4315,7 +4311,7 @@
         <v>128</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C1" s="8"/>
     </row>
@@ -4324,7 +4320,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C2" s="8"/>
     </row>
@@ -4333,16 +4329,16 @@
         <v>129</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="17" t="s">
         <v>269</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -4391,28 +4387,26 @@
         <v>133</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="D7" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>274</v>
-      </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="15" t="s">
-        <v>275</v>
-      </c>
+      <c r="G7" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>128</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C10" s="8"/>
     </row>
@@ -4421,7 +4415,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C11" s="8"/>
       <c r="F11" s="8"/>
@@ -4431,13 +4425,13 @@
         <v>129</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>278</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4480,13 +4474,13 @@
         <v>133</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>282</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4494,7 +4488,7 @@
         <v>128</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C18" s="8"/>
     </row>
@@ -4503,7 +4497,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C19" s="8"/>
     </row>
@@ -4515,10 +4509,10 @@
         <v>51</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -4563,13 +4557,13 @@
         <v>133</v>
       </c>
       <c r="B24" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>288</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4606,10 +4600,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -4617,19 +4611,19 @@
         <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E2" t="s">
         <v>149</v>
       </c>
       <c r="F2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -4691,27 +4685,27 @@
         <v>133</v>
       </c>
       <c r="B6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" t="s">
         <v>204</v>
       </c>
-      <c r="C6" t="s">
-        <v>205</v>
-      </c>
       <c r="D6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E6" t="s">
         <v>299</v>
       </c>
-      <c r="E6" t="s">
-        <v>301</v>
-      </c>
       <c r="F6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -4763,15 +4757,15 @@
         <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -4800,10 +4794,10 @@
         <v>154</v>
       </c>
       <c r="I16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K16" t="s">
         <v>157</v>
@@ -4973,10 +4967,10 @@
         <v>170</v>
       </c>
       <c r="I20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J20" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K20" t="s">
         <v>173</v>

</xml_diff>

<commit_message>
finish half the pages
</commit_message>
<xml_diff>
--- a/table_details/table_details_all.xlsx
+++ b/table_details/table_details_all.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BDF987-72BB-490E-8F8D-6917B22FF9A6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1-5" sheetId="2" r:id="rId1"/>
@@ -16,9 +15,9 @@
     <sheet name="24-26" sheetId="10" r:id="rId6"/>
     <sheet name="View(1-3)" sheetId="11" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="309">
   <si>
     <t>表名：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1389,12 +1388,24 @@
     <t>recommend_results</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>requirement_details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rr_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requirement_info_view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1576,7 +1587,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1611,7 +1622,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1788,33 +1799,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
-    <col min="6" max="6" width="11.375" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="8" max="8" width="13.25" customWidth="1"/>
-    <col min="10" max="10" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1822,7 +1833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1830,7 +1841,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1868,7 +1879,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1903,7 +1914,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1911,7 +1922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1946,7 +1957,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1981,10 +1992,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1992,7 +2003,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2000,7 +2011,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -2011,7 +2022,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2022,7 +2033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2030,7 +2041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2041,7 +2052,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -2052,10 +2063,10 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2063,7 +2074,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -2071,7 +2082,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -2109,7 +2120,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2147,7 +2158,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -2170,7 +2181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2208,7 +2219,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2246,7 +2257,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="6" t="s">
         <v>0</v>
       </c>
@@ -2254,7 +2265,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
@@ -2262,7 +2273,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2282,7 +2293,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2302,12 +2313,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -2327,7 +2338,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -2347,7 +2358,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2355,7 +2366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="5" t="s">
         <v>49</v>
       </c>
@@ -2363,7 +2374,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -2377,7 +2388,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -2391,7 +2402,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2399,7 +2410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -2413,7 +2424,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -2430,16 +2441,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22:L22 B38 B6:K6 B30:F30 B14:C14" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22:L22 B38 B6:K6 B30:F30 B14:C14">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:D36 B20:L20 B4:E4 G4:K4 B28:F28 B12:C12" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:D36 B20:L20 B4:E4 G4:K4 B28:F28 B12:C12">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38:D38" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38:D38">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{A0B6BE8E-FC8B-471C-84BE-24CFF94A9FEA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2449,19 +2460,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2469,7 +2480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2477,7 +2488,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2491,7 +2502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2505,7 +2516,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2513,7 +2524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2527,7 +2538,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2541,7 +2552,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2549,7 +2560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
@@ -2557,7 +2568,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -2571,7 +2582,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2585,7 +2596,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2593,7 +2604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2607,7 +2618,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -2621,7 +2632,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2629,7 +2640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
         <v>49</v>
       </c>
@@ -2637,7 +2648,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -2657,7 +2668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2677,7 +2688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -2685,7 +2696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2705,7 +2716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2725,7 +2736,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="5" t="s">
         <v>69</v>
       </c>
@@ -2733,7 +2744,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
@@ -2741,7 +2752,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2755,7 +2766,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2769,7 +2780,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -2777,7 +2788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -2791,7 +2802,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -2808,13 +2819,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B14 B22 B30:D30 D22 D14 D6 F22" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B14 B22 B30:D30 D22 D14 D6 F22">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:D12 B28:D28 B20:F20 B4:D4" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:D12 B28:D28 B20:F20 B4:D4">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 E22 C22 C6" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 E22 C22 C6">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2823,29 +2834,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92048D4E-400A-4C99-98D4-96FDDBC09EAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="18.625" customWidth="1"/>
-    <col min="2" max="2" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2853,7 +2864,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -2861,7 +2872,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2872,7 +2883,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2883,12 +2894,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2899,7 +2910,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2910,10 +2921,10 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2922,7 +2933,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2931,7 +2942,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -2942,7 +2953,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2953,12 +2964,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2969,7 +2980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -2980,7 +2991,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2988,7 +2999,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2996,7 +3007,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -3046,7 +3057,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -3096,7 +3107,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -3125,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -3175,7 +3186,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -3225,7 +3236,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -3233,7 +3244,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -3241,7 +3252,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -3252,7 +3263,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -3263,7 +3274,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -3271,7 +3282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -3282,7 +3293,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -3293,7 +3304,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -3301,7 +3312,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -3309,7 +3320,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -3320,7 +3331,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -3331,7 +3342,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -3339,7 +3350,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -3350,7 +3361,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -3361,7 +3372,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -3369,7 +3380,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -3377,7 +3388,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
@@ -3388,7 +3399,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
@@ -3399,7 +3410,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -3407,7 +3418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
@@ -3418,7 +3429,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -3432,13 +3443,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L20" xr:uid="{6AF3EB75-9AB4-4D25-870E-B1E1D91C1566}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L20">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4 B28:C28 B36:C36 B44:C44 M20:P20 B20:K20 B12:C12" xr:uid="{5F2589E5-390C-42E2-B3EB-32EDCEB3C623}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4 B28:C28 B36:C36 B44:C44 M20:P20 B20:K20 B12:C12">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 B30:C30 B38:C38 B46:C46 B22:P22 B14:C14" xr:uid="{042C3C6D-321F-4B93-A50F-35A79A2BEC25}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 B30:C30 B38:C38 B46:C46 B22:P22 B14:C14">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3447,26 +3458,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D6809F-1A5A-41FB-870C-741234E0C666}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="11.875" customWidth="1"/>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="1" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.25" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3474,7 +3485,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -3482,7 +3493,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3493,7 +3504,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3504,7 +3515,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3512,7 +3523,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3523,7 +3534,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -3534,7 +3545,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -3543,7 +3554,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -3551,7 +3562,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -3580,7 +3591,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -3609,12 +3620,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -3643,7 +3654,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -3672,7 +3683,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -3680,7 +3691,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -3689,7 +3700,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -3706,7 +3717,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -3723,12 +3734,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -3745,7 +3756,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -3762,7 +3773,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -3770,7 +3781,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -3778,7 +3789,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -3789,7 +3800,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -3800,7 +3811,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -3808,7 +3819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -3819,7 +3830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -3833,10 +3844,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:E24 B15:I15 B32:C32 B6:C6" xr:uid="{9F5C3E75-CB6F-4BAE-94EE-4069DB47DC7C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:E24 B15:I15 B32:C32 B6:C6">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:C30 B13:I13 B22:E22 B4:C4" xr:uid="{4CCE52F2-DBFC-47D5-BEE0-160A32FC4C8F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:C30 B13:I13 B22:E22 B4:C4">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3845,27 +3856,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70F3BA1-9592-4700-A3FB-45635F483D0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="14.75" style="9" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="9" customWidth="1"/>
     <col min="5" max="5" width="11" style="9" customWidth="1"/>
-    <col min="6" max="6" width="11.375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8.875" style="9"/>
-    <col min="8" max="8" width="12.375" style="9" customWidth="1"/>
-    <col min="9" max="16384" width="8.875" style="9"/>
+    <col min="6" max="6" width="11.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="9"/>
+    <col min="8" max="8" width="12.33203125" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="8" t="s">
         <v>128</v>
       </c>
@@ -3874,7 +3885,7 @@
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="13.5" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
@@ -3885,7 +3896,7 @@
       <c r="D2" s="11"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="13.95" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>129</v>
       </c>
@@ -3898,7 +3909,7 @@
       <c r="D3" s="11"/>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="13.95" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>130</v>
       </c>
@@ -3911,14 +3922,14 @@
       <c r="D4" s="11"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="13.95" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>131</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="13.95" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>132</v>
       </c>
@@ -3929,7 +3940,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="13.95" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>133</v>
       </c>
@@ -3940,7 +3951,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="8" t="s">
         <v>128</v>
       </c>
@@ -3949,7 +3960,7 @@
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
@@ -3958,7 +3969,7 @@
       </c>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="13" t="s">
         <v>129</v>
       </c>
@@ -3993,7 +4004,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="13" t="s">
         <v>130</v>
       </c>
@@ -4028,7 +4039,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="13" t="s">
         <v>131</v>
       </c>
@@ -4036,7 +4047,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="13" t="s">
         <v>132</v>
       </c>
@@ -4071,7 +4082,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="13" t="s">
         <v>133</v>
       </c>
@@ -4106,7 +4117,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="8" t="s">
         <v>128</v>
       </c>
@@ -4115,7 +4126,7 @@
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="10" t="s">
         <v>46</v>
       </c>
@@ -4124,7 +4135,7 @@
       </c>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="13" t="s">
         <v>129</v>
       </c>
@@ -4137,7 +4148,7 @@
       <c r="F21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="13" t="s">
         <v>130</v>
       </c>
@@ -4148,7 +4159,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="13" t="s">
         <v>131</v>
       </c>
@@ -4157,7 +4168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="13" t="s">
         <v>132</v>
       </c>
@@ -4168,7 +4179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="13" t="s">
         <v>133</v>
       </c>
@@ -4180,10 +4191,10 @@
       </c>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="8" t="s">
         <v>128</v>
       </c>
@@ -4192,7 +4203,7 @@
       </c>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="10" t="s">
         <v>46</v>
       </c>
@@ -4201,7 +4212,7 @@
       </c>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="13" t="s">
         <v>129</v>
       </c>
@@ -4215,7 +4226,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="13" t="s">
         <v>130</v>
       </c>
@@ -4229,14 +4240,14 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="13" t="s">
         <v>131</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="13" t="s">
         <v>132</v>
       </c>
@@ -4250,7 +4261,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="13" t="s">
         <v>133</v>
       </c>
@@ -4264,7 +4275,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -4272,16 +4283,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4 B22:C22 B30:D30 B13:F13 H13:K13" xr:uid="{8E5D7487-CF97-464D-9562-DB2B527406BB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4 B22:C22 B30:D30 B13:F13 H13:K13">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15:D15 B32 B24 F15:K15" xr:uid="{D1C12543-0413-4FFA-9D76-746A43FB4CF6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15:D15 B32 B24 F15:K15">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C32:D32 C24 E15" xr:uid="{970DC511-966C-45B6-87D7-BA5ADB48D357}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C32:D32 C24 E15">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13" xr:uid="{BA2A014C-EB16-4549-A2DB-B383B8A25FCF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4290,23 +4301,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F506D6B7-3E6F-45FA-91C1-7913AE5D78D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="9"/>
-    <col min="2" max="2" width="11.125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.75" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="11.109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
         <v>128</v>
       </c>
@@ -4315,7 +4326,7 @@
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="13.5" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
@@ -4324,7 +4335,7 @@
       </c>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="13.95" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>129</v>
       </c>
@@ -4341,7 +4352,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="13.95" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>130</v>
       </c>
@@ -4358,14 +4369,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="13.95" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>131</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="13.95" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>132</v>
       </c>
@@ -4382,7 +4393,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="13.95" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>133</v>
       </c>
@@ -4401,7 +4412,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="8" t="s">
         <v>128</v>
       </c>
@@ -4410,7 +4421,7 @@
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
@@ -4420,7 +4431,7 @@
       <c r="C11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="13" t="s">
         <v>129</v>
       </c>
@@ -4434,7 +4445,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="13" t="s">
         <v>130</v>
       </c>
@@ -4448,14 +4459,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="13" t="s">
         <v>131</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="13" t="s">
         <v>132</v>
       </c>
@@ -4469,7 +4480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="13" t="s">
         <v>133</v>
       </c>
@@ -4483,7 +4494,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="8" t="s">
         <v>128</v>
       </c>
@@ -4492,7 +4503,7 @@
       </c>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="10" t="s">
         <v>46</v>
       </c>
@@ -4501,7 +4512,7 @@
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="13" t="s">
         <v>129</v>
       </c>
@@ -4515,7 +4526,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="13" t="s">
         <v>130</v>
       </c>
@@ -4529,7 +4540,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="13" t="s">
         <v>131</v>
       </c>
@@ -4538,7 +4549,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="13" t="s">
         <v>132</v>
       </c>
@@ -4552,7 +4563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="13" t="s">
         <v>133</v>
       </c>
@@ -4569,13 +4580,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 C15:D15 C23:D23" xr:uid="{9FE8C4B3-8378-4985-99C5-079CAE9C53D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 C15:D15 C23:D23">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E6 B15 B23" xr:uid="{4605203D-75CF-4343-B8B0-E907ED628E06}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E6 B15 B23">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:D13 B4:E4 B21:D21" xr:uid="{DD3CF57C-BCF2-4845-A8D9-7E46E070E1C0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:D13 B4:E4 B21:D21">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4584,21 +4595,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D6CB52-9EB7-455C-8F84-F35A52C5F1B4}">
-  <dimension ref="A1:O20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:O20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>294</v>
       </c>
@@ -4606,7 +4618,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" s="13" t="s">
         <v>129</v>
       </c>
@@ -4626,7 +4638,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="13" t="s">
         <v>130</v>
       </c>
@@ -4646,7 +4658,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="13" t="s">
         <v>131</v>
       </c>
@@ -4660,7 +4672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="A5" s="13" t="s">
         <v>132</v>
       </c>
@@ -4680,7 +4692,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" s="13" t="s">
         <v>133</v>
       </c>
@@ -4700,7 +4712,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" s="15" t="s">
         <v>294</v>
       </c>
@@ -4708,7 +4720,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -4719,7 +4731,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -4730,7 +4742,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -4738,7 +4750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -4749,7 +4761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -4760,7 +4772,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15">
       <c r="A15" s="15" t="s">
         <v>294</v>
       </c>
@@ -4768,7 +4780,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -4815,7 +4827,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -4862,7 +4874,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -4894,7 +4906,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -4941,7 +4953,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -4986,21 +4998,367 @@
       </c>
       <c r="O20" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" t="s">
+        <v>78</v>
+      </c>
+      <c r="K23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" t="s">
+        <v>92</v>
+      </c>
+      <c r="N23" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O24" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P24" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>20</v>
+      </c>
+      <c r="J25">
+        <v>20</v>
+      </c>
+      <c r="M25">
+        <v>20</v>
+      </c>
+      <c r="O25" s="15">
+        <v>20</v>
+      </c>
+      <c r="P25" s="9"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>307</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" t="s">
+        <v>80</v>
+      </c>
+      <c r="K27" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" t="s">
+        <v>82</v>
+      </c>
+      <c r="M27" t="s">
+        <v>93</v>
+      </c>
+      <c r="N27" t="s">
+        <v>91</v>
+      </c>
+      <c r="O27" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="P27" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+      <c r="F32" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:F3 B10:C10 M17:O17 B17:K17" xr:uid="{672A8DB7-17F9-4041-9274-565953294B28}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:G26 K26 N26 Q26 P33 M33 J33 B33 B5:F5 B12 B19:O19 B26:D26">
+      <formula1>"k,m,k&amp;m,n"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:J26 L26:M26 O26:P26 E26 C33:I33 N33:O33 K33:L33 C12">
+      <formula1>"k,m,k&amp;m"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:F3 B31:P31 B10:C10 M17:O17 B17:K17 B24:Q24">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:F5 B12 B19:O19" xr:uid="{46A27783-6485-4EF8-89C7-A4A0624C58E8}">
-      <formula1>"k,m,k&amp;m,n"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{60417A34-0ECB-4D94-89CD-F63C40054958}">
-      <formula1>"k,m,k&amp;m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L17" xr:uid="{6BC1AFAF-92C1-4FFF-9FDF-59CE7671F298}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L17">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add a view `requirement_list`&fix a bug in table_details_all
- addd a view `requirement_list` for page Quire_Recruit_HR
- fix the bug that rr_sta_id doesn't exist in table_details_all,the
column had been added to the table in earlier commit
</commit_message>
<xml_diff>
--- a/table_details/table_details_all.xlsx
+++ b/table_details/table_details_all.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13009D38-7063-47C4-B96A-44E07C646DC3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-5" sheetId="2" r:id="rId1"/>
@@ -13,11 +14,11 @@
     <sheet name="16-19" sheetId="8" r:id="rId4"/>
     <sheet name="20-23" sheetId="9" r:id="rId5"/>
     <sheet name="24-26" sheetId="10" r:id="rId6"/>
-    <sheet name="View(1-3)" sheetId="11" r:id="rId7"/>
+    <sheet name="View(1-5)" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="311">
   <si>
     <t>表名：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -502,10 +503,6 @@
   </si>
   <si>
     <t>rr_ri_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求的推荐</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1400,12 +1397,24 @@
     <t>requirement_info_view</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>需求的处理阶段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rr_sta_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requirement_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1799,33 +1808,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.25" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="11.125" customWidth="1"/>
+    <col min="6" max="6" width="11.375" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="13.25" customWidth="1"/>
+    <col min="10" max="10" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1833,7 +1842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1841,7 +1850,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1876,10 +1885,10 @@
         <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1913,8 +1922,11 @@
       <c r="K4" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="L4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1922,7 +1934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1956,8 +1968,11 @@
       <c r="K6" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1991,38 +2006,41 @@
       <c r="K7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="L7" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>290</v>
+      </c>
+      <c r="C11" t="s">
         <v>291</v>
       </c>
-      <c r="C11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2033,7 +2051,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2041,7 +2059,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2052,21 +2070,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" t="s">
         <v>134</v>
       </c>
-      <c r="C15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2074,7 +2092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -2082,7 +2100,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2138,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2158,7 +2176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -2181,7 +2199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2219,7 +2237,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2257,7 +2275,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>0</v>
       </c>
@@ -2265,7 +2283,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
@@ -2273,7 +2291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2293,7 +2311,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2313,12 +2331,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -2338,7 +2356,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -2358,7 +2376,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2366,7 +2384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>49</v>
       </c>
@@ -2374,7 +2392,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -2388,7 +2406,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -2402,7 +2420,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2410,7 +2428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -2424,7 +2442,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -2441,16 +2459,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22:L22 B38 B6:K6 B30:F30 B14:C14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22:L22 B38 B6:L6 B30:F30 B14:C14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:D36 B20:L20 B4:E4 G4:K4 B28:F28 B12:C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:D36 B20:L20 B4:E4 G4:L4 B28:F28 B12:C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38:D38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38:D38" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2460,19 +2478,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2480,7 +2498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2488,7 +2506,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2502,7 +2520,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2516,7 +2534,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2524,7 +2542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2538,7 +2556,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2552,7 +2570,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2560,7 +2578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
@@ -2568,7 +2586,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -2582,7 +2600,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2596,7 +2614,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2604,7 +2622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2618,7 +2636,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -2632,7 +2650,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2640,7 +2658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>49</v>
       </c>
@@ -2648,7 +2666,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -2668,7 +2686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2688,7 +2706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -2696,7 +2714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2716,7 +2734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2736,7 +2754,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>69</v>
       </c>
@@ -2744,7 +2762,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
@@ -2752,7 +2770,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2766,7 +2784,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2780,7 +2798,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -2788,7 +2806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -2802,7 +2820,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -2819,13 +2837,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B14 B22 B30:D30 D22 D14 D6 F22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B14 B22 B30:D30 D22 D14 D6 F22" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:D12 B28:D28 B20:F20 B4:D4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:D12 B28:D28 B20:F20 B4:D4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 E22 C22 C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 E22 C22 C6" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2834,56 +2852,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
+    <col min="2" max="2" width="9.625" customWidth="1"/>
     <col min="3" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
         <v>138</v>
       </c>
-      <c r="C3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2894,12 +2912,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2910,39 +2928,39 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
         <v>140</v>
       </c>
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -2950,10 +2968,10 @@
         <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2964,12 +2982,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2980,84 +2998,84 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" t="s">
         <v>144</v>
       </c>
-      <c r="C15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
         <v>148</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>149</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>150</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>151</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>152</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>153</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>154</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>155</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>156</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>157</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>158</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>159</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>160</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>161</v>
       </c>
-      <c r="P19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -3107,7 +3125,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -3136,12 +3154,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>29</v>
@@ -3186,84 +3204,84 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" t="s">
         <v>164</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>165</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>166</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>167</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>168</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>169</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>170</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>171</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>172</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>173</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>174</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>175</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>176</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>177</v>
       </c>
-      <c r="P23" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27" t="s">
         <v>180</v>
       </c>
-      <c r="C27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -3274,7 +3292,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -3282,7 +3300,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -3293,45 +3311,45 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B31" t="s">
+        <v>181</v>
+      </c>
+      <c r="C31" t="s">
         <v>182</v>
       </c>
-      <c r="C31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>185</v>
+      </c>
+      <c r="C35" t="s">
         <v>186</v>
       </c>
-      <c r="C35" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -3342,7 +3360,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -3350,7 +3368,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -3361,45 +3379,45 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B39" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" t="s">
         <v>188</v>
       </c>
-      <c r="C39" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" t="s">
         <v>192</v>
       </c>
-      <c r="C43" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
@@ -3410,7 +3428,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -3418,7 +3436,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
@@ -3429,27 +3447,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B47" t="s">
+        <v>193</v>
+      </c>
+      <c r="C47" t="s">
         <v>194</v>
-      </c>
-      <c r="C47" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L20" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4 B28:C28 B36:C36 B44:C44 M20:P20 B20:K20 B12:C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4 B28:C28 B36:C36 B44:C44 M20:P20 B20:K20 B12:C12" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 B30:C30 B38:C38 B46:C46 B22:P22 B14:C14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 B30:C30 B38:C38 B46:C46 B22:P22 B14:C14" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3458,53 +3476,53 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="1" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="11.375" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
         <v>124</v>
       </c>
-      <c r="C3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3515,7 +3533,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3523,7 +3541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3534,64 +3552,64 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" t="s">
         <v>126</v>
       </c>
-      <c r="C7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C12" t="s">
         <v>110</v>
       </c>
       <c r="D12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" t="s">
         <v>199</v>
       </c>
-      <c r="E12" t="s">
-        <v>148</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" t="s">
         <v>200</v>
       </c>
-      <c r="G12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>201</v>
       </c>
-      <c r="I12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -3620,12 +3638,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -3654,70 +3672,70 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" t="s">
         <v>203</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>204</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>205</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>206</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>207</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>208</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>209</v>
       </c>
-      <c r="I16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" t="s">
         <v>213</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>214</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>215</v>
       </c>
-      <c r="E21" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -3734,12 +3752,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -3756,51 +3774,51 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B25" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" t="s">
         <v>217</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>218</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>219</v>
       </c>
-      <c r="E25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C29" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -3811,7 +3829,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -3819,7 +3837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -3830,24 +3848,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B33" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" t="s">
         <v>224</v>
-      </c>
-      <c r="C33" t="s">
-        <v>225</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:E24 B15:I15 B32:C32 B6:C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:E24 B15:I15 B32:C32 B6:C6" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:C30 B13:I13 B22:E22 B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:C30 B13:I13 B22:E22 B4:C4" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3856,62 +3874,62 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="14.75" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="9.625" style="9" customWidth="1"/>
     <col min="5" max="5" width="11" style="9" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="9"/>
-    <col min="8" max="8" width="12.33203125" style="9" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="9"/>
+    <col min="6" max="6" width="11.375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="9"/>
+    <col min="8" max="8" width="12.375" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="8.875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:11" ht="13.5" customHeight="1">
+    <row r="2" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="11"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:11" ht="13.95" customHeight="1">
+    <row r="3" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>229</v>
       </c>
       <c r="D3" s="11"/>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:11" ht="13.95" customHeight="1">
+    <row r="4" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>5</v>
@@ -3922,16 +3940,16 @@
       <c r="D4" s="11"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:11" ht="13.95" customHeight="1">
+    <row r="5" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="13.95" customHeight="1">
+    <row r="6" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>27</v>
@@ -3940,73 +3958,73 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13.95" customHeight="1">
+    <row r="7" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="16" t="s">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>232</v>
-      </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="13" t="s">
+      <c r="C12" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>26</v>
@@ -4039,17 +4057,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>27</v>
@@ -4082,75 +4100,75 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="F16" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="G16" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H16" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="I16" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="J16" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="K16" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="K16" s="17" t="s">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>252</v>
-      </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>253</v>
-      </c>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="F21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>5</v>
@@ -4159,18 +4177,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>27</v>
@@ -4179,56 +4197,56 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>257</v>
-      </c>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="13" t="s">
+      <c r="D29" s="17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>39</v>
@@ -4240,16 +4258,16 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>27</v>
@@ -4261,21 +4279,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="D33" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -4283,16 +4301,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4 B22:C22 B30:D30 B13:F13 H13:K13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4 B22:C22 B30:D30 B13:F13 H13:K13" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15:D15 B32 B24 F15:K15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15:D15 B32 B24 F15:K15" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C32:D32 C24 E15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C32:D32 C24 E15" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4301,60 +4319,60 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="11.109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.875" style="9"/>
+    <col min="2" max="2" width="11.125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="12.125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.75" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="13.5" customHeight="1">
+    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="13.95" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="C3" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="13.95" customHeight="1">
-      <c r="A4" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>26</v>
@@ -4369,16 +4387,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.95" customHeight="1">
+    <row r="5" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="13.95" customHeight="1">
+    <row r="6" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>27</v>
@@ -4393,61 +4411,61 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.95" customHeight="1">
+    <row r="7" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="D7" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="17" t="s">
         <v>272</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>273</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>5</v>
@@ -4459,16 +4477,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>27</v>
@@ -4480,55 +4498,55 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="D16" s="17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>282</v>
-      </c>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>39</v>
@@ -4540,18 +4558,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>27</v>
@@ -4563,30 +4581,30 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="D24" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 C15:D15 C23:D23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 C15:D15 C23:D23" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E6 B15 B23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E6 B15 B23" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:D13 B4:E4 B21:D21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:D13 B4:E4 B21:D21" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4595,52 +4613,52 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" t="s">
         <v>294</v>
       </c>
-      <c r="B1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
         <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -4658,9 +4676,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -4672,9 +4690,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
@@ -4692,35 +4710,35 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" t="s">
         <v>203</v>
       </c>
-      <c r="C6" t="s">
-        <v>204</v>
-      </c>
       <c r="D6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" t="s">
         <v>297</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" t="s">
         <v>299</v>
       </c>
-      <c r="F6" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="B8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -4731,7 +4749,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -4742,7 +4760,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -4750,7 +4768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -4761,7 +4779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -4769,65 +4787,65 @@
         <v>55</v>
       </c>
       <c r="C13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="B15" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
         <v>148</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>149</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>150</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>151</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>152</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>153</v>
       </c>
-      <c r="H16" t="s">
-        <v>154</v>
-      </c>
       <c r="I16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K16" t="s">
+        <v>156</v>
+      </c>
+      <c r="L16" t="s">
         <v>157</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>158</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>159</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>160</v>
       </c>
-      <c r="O16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -4874,7 +4892,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -4906,12 +4924,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>29</v>
@@ -4953,62 +4971,62 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" t="s">
         <v>164</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>165</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>166</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>167</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>168</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>169</v>
       </c>
-      <c r="H20" t="s">
-        <v>170</v>
-      </c>
       <c r="I20" t="s">
+        <v>302</v>
+      </c>
+      <c r="J20" t="s">
         <v>303</v>
       </c>
-      <c r="J20" t="s">
-        <v>304</v>
-      </c>
       <c r="K20" t="s">
+        <v>172</v>
+      </c>
+      <c r="L20" t="s">
         <v>173</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>174</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>175</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>176</v>
       </c>
-      <c r="O20" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -5052,16 +5070,16 @@
         <v>24</v>
       </c>
       <c r="O23" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="P23" s="17" t="s">
         <v>284</v>
-      </c>
-      <c r="P23" s="17" t="s">
-        <v>285</v>
       </c>
       <c r="Q23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -5114,7 +5132,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -5138,12 +5156,12 @@
       </c>
       <c r="P25" s="9"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>29</v>
@@ -5191,12 +5209,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
@@ -5235,24 +5253,24 @@
         <v>91</v>
       </c>
       <c r="O27" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="P27" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="P27" s="17" t="s">
-        <v>288</v>
       </c>
       <c r="Q27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B29" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -5269,10 +5287,10 @@
         <v>34</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -5292,7 +5310,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -5306,7 +5324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -5326,7 +5344,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -5343,22 +5361,175 @@
         <v>82</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B36" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" t="s">
+        <v>78</v>
+      </c>
+      <c r="I37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>20</v>
+      </c>
+      <c r="G39">
+        <v>20</v>
+      </c>
+      <c r="H39">
+        <v>20</v>
+      </c>
+      <c r="I39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>87</v>
+      </c>
+      <c r="G41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H41" t="s">
+        <v>80</v>
+      </c>
+      <c r="I41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:G26 K26 N26 Q26 P33 M33 J33 B33 B5:F5 B12 B19:O19 B26:D26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:G26 K26 N26 P33 M33 J33 B33 B5:F5 B12 B19:O19 B26:D26 B40:E40 Q26 I40:J40" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:J26 L26:M26 O26:P26 E26 C33:I33 N33:O33 K33:L33 C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:J26 L26:M26 O26:P26 E26 C33:I33 N33:O33 K33:L33 C12 F40:H40" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:F3 B31:P31 B10:C10 M17:O17 B17:K17 B24:Q24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:F3 B31:P31 B10:C10 M17:O17 B17:K17 B24:Q24 B38:H38 J38" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L17 I38" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add view of recommend_notify
</commit_message>
<xml_diff>
--- a/table_details/table_details_all.xlsx
+++ b/table_details/table_details_all.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AADE457-B3A4-4731-A7F2-BC156AA61252}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF534C81-92F7-429E-B28B-20559E60ED90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
     <sheet name="10-15" sheetId="7" r:id="rId4"/>
     <sheet name="20-23" sheetId="9" r:id="rId5"/>
     <sheet name="24-26" sheetId="10" r:id="rId6"/>
-    <sheet name="View(1-5)" sheetId="11" r:id="rId7"/>
+    <sheet name="View(1-7)" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="314">
   <si>
     <t>表名：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1412,6 +1412,14 @@
   </si>
   <si>
     <t>SRM系列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recommend_notify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recstu_email</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1823,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2486,7 +2494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:B15"/>
     </sheetView>
   </sheetViews>
@@ -2860,8 +2868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3258,8 +3266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3882,7 +3890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4619,10 +4627,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5537,16 +5545,115 @@
         <v>308</v>
       </c>
     </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B43" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" t="s">
+        <v>198</v>
+      </c>
+      <c r="D44" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>20</v>
+      </c>
+      <c r="F46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>202</v>
+      </c>
+      <c r="C48" t="s">
+        <v>204</v>
+      </c>
+      <c r="D48" t="s">
+        <v>205</v>
+      </c>
+      <c r="E48" t="s">
+        <v>313</v>
+      </c>
+      <c r="F48" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:G26 K26 N26 P33 M33 J33 B33 B5:G5 B12 B19:O19 B26:D26 B40:E40 Q26 I40:J40" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:G26 K26 N26 P33 M33 J33 B33 B5:G5 B12 B19:O19 B26:D26 B40:E40 Q26 I40:J40 B47:F47" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:J26 L26:M26 O26:P26 E26 C33:I33 N33:O33 K33:L33 C12 F40:H40" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>"k,m,k&amp;m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3 B31:P31 B10:C10 M17:O17 B17:K17 B24:Q24 B38:H38 J38" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3 B31:P31 B10:C10 M17:O17 B17:K17 B24:Q24 B38:H38 J38 B45:F45" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L17 I38" xr:uid="{00000000-0002-0000-0600-000003000000}">

</xml_diff>